<commit_message>
More work on results description
</commit_message>
<xml_diff>
--- a/calibration/table1_concentric_vs_dipole.xlsx
+++ b/calibration/table1_concentric_vs_dipole.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE650AEC-4545-4AC6-8137-1B36C5DCE93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FDCA44-9479-4DDA-9F26-7D5BAC958CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14625" yWindow="7350" windowWidth="13245" windowHeight="7830" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="11580" yWindow="1155" windowWidth="13245" windowHeight="7830" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -174,15 +175,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -194,12 +186,21 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -265,6 +266,60 @@
           </cell>
           <cell r="I6">
             <v>57.214955496532816</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="B4">
+            <v>0.60341407173788841</v>
+          </cell>
+          <cell r="C4">
+            <v>1.239157480346315</v>
+          </cell>
+          <cell r="D4">
+            <v>0.28266276411689345</v>
+          </cell>
+          <cell r="E4">
+            <v>0.60700827065986507</v>
+          </cell>
+          <cell r="F4">
+            <v>0.63368086621699915</v>
+          </cell>
+          <cell r="G4">
+            <v>1.3879593516431761</v>
+          </cell>
+          <cell r="H4">
+            <v>0.28266276411689345</v>
+          </cell>
+          <cell r="I4">
+            <v>0.60700827065986507</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>0.7291301197349368</v>
+          </cell>
+          <cell r="C7">
+            <v>1.5313548892358326</v>
+          </cell>
+          <cell r="D7">
+            <v>0.51668648837242548</v>
+          </cell>
+          <cell r="E7">
+            <v>1.4845454261428004</v>
           </cell>
         </row>
       </sheetData>
@@ -573,7 +628,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,142 +637,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="5">
         <f>[1]Sheet1!F4</f>
         <v>0.3220060130641641</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="5">
         <f>[1]Sheet1!G4</f>
         <v>0.82834158000689395</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="5">
         <f>[1]Sheet1!H4</f>
         <v>0.28005355875987198</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <f>[1]Sheet1!I4</f>
         <v>0.64031875255130177</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="F4" s="7">
+        <f>[2]Sheet1!F4</f>
+        <v>0.63368086621699915</v>
+      </c>
+      <c r="G4" s="7">
+        <f>[2]Sheet1!G4</f>
+        <v>1.3879593516431761</v>
+      </c>
+      <c r="H4" s="7">
+        <f>[2]Sheet1!H4</f>
+        <v>0.28266276411689345</v>
+      </c>
+      <c r="I4" s="7">
+        <f>[2]Sheet1!I4</f>
+        <v>0.60700827065986507</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="5">
         <f>[1]Sheet1!B4</f>
         <v>0.20169901228894177</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <f>[1]Sheet1!C4</f>
         <v>0.45445095085292847</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="5">
         <f>[1]Sheet1!D4</f>
         <v>0.28005355875987198</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <f>[1]Sheet1!E4</f>
         <v>0.64031875255130177</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="F5" s="7">
+        <f>[2]Sheet1!B4</f>
+        <v>0.60341407173788841</v>
+      </c>
+      <c r="G5" s="7">
+        <f>[2]Sheet1!C4</f>
+        <v>1.239157480346315</v>
+      </c>
+      <c r="H5" s="7">
+        <f>[2]Sheet1!D4</f>
+        <v>0.28266276411689345</v>
+      </c>
+      <c r="I5" s="7">
+        <f>[2]Sheet1!E4</f>
+        <v>0.60700827065986507</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="8">
         <f>[1]Sheet1!F6</f>
         <v>28.25890846273203</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <f>[1]Sheet1!G6</f>
         <v>73.798305452756779</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <f>[1]Sheet1!H6</f>
         <v>20.134911477692057</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <f>[1]Sheet1!I6</f>
         <v>57.214955496532816</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="F6" s="7">
+        <f>[2]Sheet1!B7</f>
+        <v>0.7291301197349368</v>
+      </c>
+      <c r="G6" s="7">
+        <f>[2]Sheet1!C7</f>
+        <v>1.5313548892358326</v>
+      </c>
+      <c r="H6" s="7">
+        <f>[2]Sheet1!D7</f>
+        <v>0.51668648837242548</v>
+      </c>
+      <c r="I6" s="7">
+        <f>[2]Sheet1!E7</f>
+        <v>1.4845454261428004</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K12" s="2"/>

</xml_diff>

<commit_message>
Updated table I and II, moving the test output .xlsx files here so that there are no links out from this directory.
</commit_message>
<xml_diff>
--- a/calibration/table1_concentric_vs_dipole.xlsx
+++ b/calibration/table1_concentric_vs_dipole.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FDCA44-9479-4DDA-9F26-7D5BAC958CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA215B3-0C6A-4326-A4A4-42AB3BDF999B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="1155" windowWidth="13245" windowHeight="7830" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="8196" yWindow="18864" windowWidth="14988" windowHeight="6792" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -175,34 +175,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,51 +224,55 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet1"/>
+      <sheetName val="Error stats"/>
+      <sheetName val="Residue stats"/>
+      <sheetName val="Cal stats"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="4">
           <cell r="B4">
-            <v>0.20169901228894177</v>
+            <v>0.2019826251213456</v>
           </cell>
           <cell r="C4">
-            <v>0.45445095085292847</v>
+            <v>0.52530516833145802</v>
           </cell>
           <cell r="D4">
-            <v>0.28005355875987198</v>
+            <v>0.21850341771098758</v>
           </cell>
           <cell r="E4">
-            <v>0.64031875255130177</v>
+            <v>0.57728246882325973</v>
           </cell>
           <cell r="F4">
-            <v>0.3220060130641641</v>
+            <v>0.33530991217960948</v>
           </cell>
           <cell r="G4">
-            <v>0.82834158000689395</v>
+            <v>0.93119259717385872</v>
           </cell>
           <cell r="H4">
-            <v>0.28005355875987198</v>
+            <v>0.21850341771098758</v>
           </cell>
           <cell r="I4">
-            <v>0.64031875255130177</v>
+            <v>0.57728246882325973</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="F6">
-            <v>28.25890846273203</v>
-          </cell>
-          <cell r="G6">
-            <v>73.798305452756779</v>
-          </cell>
-          <cell r="H6">
-            <v>20.134911477692057</v>
-          </cell>
-          <cell r="I6">
-            <v>57.214955496532816</v>
+          <cell r="B6">
+            <v>28.304957333576017</v>
+          </cell>
+          <cell r="C6">
+            <v>73.63553983783126</v>
+          </cell>
+          <cell r="D6">
+            <v>20.272569520908039</v>
+          </cell>
+          <cell r="E6">
+            <v>56.884775449910173</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -278,51 +282,55 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet1"/>
+      <sheetName val="Error stats"/>
+      <sheetName val="Residue stats"/>
+      <sheetName val="Cal stats"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="4">
           <cell r="B4">
-            <v>0.60341407173788841</v>
+            <v>0.28344638376068243</v>
           </cell>
           <cell r="C4">
-            <v>1.239157480346315</v>
+            <v>0.76680325619476697</v>
           </cell>
           <cell r="D4">
-            <v>0.28266276411689345</v>
+            <v>0.27469341877840853</v>
           </cell>
           <cell r="E4">
-            <v>0.60700827065986507</v>
+            <v>0.64227560401111072</v>
           </cell>
           <cell r="F4">
-            <v>0.63368086621699915</v>
+            <v>0.45156805827987784</v>
           </cell>
           <cell r="G4">
-            <v>1.3879593516431761</v>
+            <v>1.3044023148183825</v>
           </cell>
           <cell r="H4">
-            <v>0.28266276411689345</v>
+            <v>0.27469341877840853</v>
           </cell>
           <cell r="I4">
-            <v>0.60700827065986507</v>
+            <v>0.64227560401111072</v>
           </cell>
         </row>
-        <row r="7">
-          <cell r="B7">
-            <v>0.7291301197349368</v>
-          </cell>
-          <cell r="C7">
-            <v>1.5313548892358326</v>
-          </cell>
-          <cell r="D7">
-            <v>0.51668648837242548</v>
-          </cell>
-          <cell r="E7">
-            <v>1.4845454261428004</v>
+        <row r="6">
+          <cell r="F6">
+            <v>0.87729002129534805</v>
+          </cell>
+          <cell r="G6">
+            <v>2.5765351802957399</v>
+          </cell>
+          <cell r="H6">
+            <v>0.51090298228368991</v>
+          </cell>
+          <cell r="I6">
+            <v>1.4147130140210986</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -628,209 +636,209 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="3" t="s">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
-        <f>[1]Sheet1!F4</f>
-        <v>0.3220060130641641</v>
-      </c>
-      <c r="C4" s="5">
-        <f>[1]Sheet1!G4</f>
-        <v>0.82834158000689395</v>
-      </c>
-      <c r="D4" s="5">
-        <f>[1]Sheet1!H4</f>
-        <v>0.28005355875987198</v>
-      </c>
-      <c r="E4" s="6">
-        <f>[1]Sheet1!I4</f>
-        <v>0.64031875255130177</v>
-      </c>
-      <c r="F4" s="7">
-        <f>[2]Sheet1!F4</f>
-        <v>0.63368086621699915</v>
-      </c>
-      <c r="G4" s="7">
-        <f>[2]Sheet1!G4</f>
-        <v>1.3879593516431761</v>
-      </c>
-      <c r="H4" s="7">
-        <f>[2]Sheet1!H4</f>
-        <v>0.28266276411689345</v>
-      </c>
-      <c r="I4" s="7">
-        <f>[2]Sheet1!I4</f>
-        <v>0.60700827065986507</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="B4" s="10">
+        <f>'[1]Error stats'!F4</f>
+        <v>0.33530991217960948</v>
+      </c>
+      <c r="C4" s="10">
+        <f>'[1]Error stats'!G4</f>
+        <v>0.93119259717385872</v>
+      </c>
+      <c r="D4" s="10">
+        <f>'[1]Error stats'!H4</f>
+        <v>0.21850341771098758</v>
+      </c>
+      <c r="E4" s="11">
+        <f>'[1]Error stats'!I4</f>
+        <v>0.57728246882325973</v>
+      </c>
+      <c r="F4" s="12">
+        <f>'[2]Error stats'!F4</f>
+        <v>0.45156805827987784</v>
+      </c>
+      <c r="G4" s="12">
+        <f>'[2]Error stats'!G4</f>
+        <v>1.3044023148183825</v>
+      </c>
+      <c r="H4" s="12">
+        <f>'[2]Error stats'!H4</f>
+        <v>0.27469341877840853</v>
+      </c>
+      <c r="I4" s="12">
+        <f>'[2]Error stats'!I4</f>
+        <v>0.64227560401111072</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
-        <f>[1]Sheet1!B4</f>
-        <v>0.20169901228894177</v>
-      </c>
-      <c r="C5" s="5">
-        <f>[1]Sheet1!C4</f>
-        <v>0.45445095085292847</v>
-      </c>
-      <c r="D5" s="5">
-        <f>[1]Sheet1!D4</f>
-        <v>0.28005355875987198</v>
-      </c>
-      <c r="E5" s="6">
-        <f>[1]Sheet1!E4</f>
-        <v>0.64031875255130177</v>
-      </c>
-      <c r="F5" s="7">
-        <f>[2]Sheet1!B4</f>
-        <v>0.60341407173788841</v>
-      </c>
-      <c r="G5" s="7">
-        <f>[2]Sheet1!C4</f>
-        <v>1.239157480346315</v>
-      </c>
-      <c r="H5" s="7">
-        <f>[2]Sheet1!D4</f>
-        <v>0.28266276411689345</v>
-      </c>
-      <c r="I5" s="7">
-        <f>[2]Sheet1!E4</f>
-        <v>0.60700827065986507</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="B5" s="10">
+        <f>'[1]Error stats'!B4</f>
+        <v>0.2019826251213456</v>
+      </c>
+      <c r="C5" s="10">
+        <f>'[1]Error stats'!C4</f>
+        <v>0.52530516833145802</v>
+      </c>
+      <c r="D5" s="10">
+        <f>'[1]Error stats'!D4</f>
+        <v>0.21850341771098758</v>
+      </c>
+      <c r="E5" s="11">
+        <f>'[1]Error stats'!E4</f>
+        <v>0.57728246882325973</v>
+      </c>
+      <c r="F5" s="12">
+        <f>'[2]Error stats'!B4</f>
+        <v>0.28344638376068243</v>
+      </c>
+      <c r="G5" s="12">
+        <f>'[2]Error stats'!C4</f>
+        <v>0.76680325619476697</v>
+      </c>
+      <c r="H5" s="12">
+        <f>'[2]Error stats'!D4</f>
+        <v>0.27469341877840853</v>
+      </c>
+      <c r="I5" s="12">
+        <f>'[2]Error stats'!E4</f>
+        <v>0.64227560401111072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8">
-        <f>[1]Sheet1!F6</f>
-        <v>28.25890846273203</v>
-      </c>
-      <c r="C6" s="7">
-        <f>[1]Sheet1!G6</f>
-        <v>73.798305452756779</v>
-      </c>
-      <c r="D6" s="7">
-        <f>[1]Sheet1!H6</f>
-        <v>20.134911477692057</v>
-      </c>
-      <c r="E6" s="6">
-        <f>[1]Sheet1!I6</f>
-        <v>57.214955496532816</v>
-      </c>
-      <c r="F6" s="7">
-        <f>[2]Sheet1!B7</f>
-        <v>0.7291301197349368</v>
-      </c>
-      <c r="G6" s="7">
-        <f>[2]Sheet1!C7</f>
-        <v>1.5313548892358326</v>
-      </c>
-      <c r="H6" s="7">
-        <f>[2]Sheet1!D7</f>
-        <v>0.51668648837242548</v>
-      </c>
-      <c r="I6" s="7">
-        <f>[2]Sheet1!E7</f>
-        <v>1.4845454261428004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="14">
+        <f>'[1]Error stats'!B6</f>
+        <v>28.304957333576017</v>
+      </c>
+      <c r="C6" s="12">
+        <f>'[1]Error stats'!C6</f>
+        <v>73.63553983783126</v>
+      </c>
+      <c r="D6" s="12">
+        <f>'[1]Error stats'!D6</f>
+        <v>20.272569520908039</v>
+      </c>
+      <c r="E6" s="11">
+        <f>'[1]Error stats'!E6</f>
+        <v>56.884775449910173</v>
+      </c>
+      <c r="F6" s="12">
+        <f>'[2]Error stats'!F6</f>
+        <v>0.87729002129534805</v>
+      </c>
+      <c r="G6" s="12">
+        <f>'[2]Error stats'!G6</f>
+        <v>2.5765351802957399</v>
+      </c>
+      <c r="H6" s="12">
+        <f>'[2]Error stats'!H6</f>
+        <v>0.51090298228368991</v>
+      </c>
+      <c r="I6" s="12">
+        <f>'[2]Error stats'!I6</f>
+        <v>1.4147130140210986</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>

</xml_diff>

<commit_message>
Added axis sweep figures, also tweaked tables to have a more compact 8 point format.
</commit_message>
<xml_diff>
--- a/calibration/table1_concentric_vs_dipole.xlsx
+++ b/calibration/table1_concentric_vs_dipole.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA215B3-0C6A-4326-A4A4-42AB3BDF999B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26138AC2-A61B-4766-BD2B-5991B6248A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8196" yWindow="18864" windowWidth="14988" windowHeight="6792" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="23532" yWindow="8784" windowWidth="15612" windowHeight="8148" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -144,11 +144,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -157,7 +159,47 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -167,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,34 +217,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,156 +704,157 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
+    <col min="2" max="9" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" s="15" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="7" t="s">
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="7">
         <f>'[1]Error stats'!F4</f>
         <v>0.33530991217960948</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="7">
         <f>'[1]Error stats'!G4</f>
         <v>0.93119259717385872</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="7">
         <f>'[1]Error stats'!H4</f>
         <v>0.21850341771098758</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="8">
         <f>'[1]Error stats'!I4</f>
         <v>0.57728246882325973</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="7">
         <f>'[2]Error stats'!F4</f>
         <v>0.45156805827987784</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="7">
         <f>'[2]Error stats'!G4</f>
         <v>1.3044023148183825</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="7">
         <f>'[2]Error stats'!H4</f>
         <v>0.27469341877840853</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="7">
         <f>'[2]Error stats'!I4</f>
         <v>0.64227560401111072</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="7">
         <f>'[1]Error stats'!B4</f>
         <v>0.2019826251213456</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="7">
         <f>'[1]Error stats'!C4</f>
         <v>0.52530516833145802</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <f>'[1]Error stats'!D4</f>
         <v>0.21850341771098758</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="8">
         <f>'[1]Error stats'!E4</f>
         <v>0.57728246882325973</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="7">
         <f>'[2]Error stats'!B4</f>
         <v>0.28344638376068243</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="7">
         <f>'[2]Error stats'!C4</f>
         <v>0.76680325619476697</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="7">
         <f>'[2]Error stats'!D4</f>
         <v>0.27469341877840853</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="7">
         <f>'[2]Error stats'!E4</f>
         <v>0.64227560401111072</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:13" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <f>'[1]Error stats'!B6</f>
         <v>28.304957333576017</v>
       </c>
@@ -797,7 +866,7 @@
         <f>'[1]Error stats'!D6</f>
         <v>20.272569520908039</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="13">
         <f>'[1]Error stats'!E6</f>
         <v>56.884775449910173</v>
       </c>
@@ -818,6 +887,7 @@
         <v>1.4147130140210986</v>
       </c>
     </row>
+    <row r="7" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>

</xml_diff>

<commit_message>
Work in calibration/ on stage uncertainty, added stage_uncertainty.xlsx.
</commit_message>
<xml_diff>
--- a/calibration/table1_concentric_vs_dipole.xlsx
+++ b/calibration/table1_concentric_vs_dipole.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26138AC2-A61B-4766-BD2B-5991B6248A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4456DB9B-AF8E-4D3D-BED1-04559590EEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23532" yWindow="8784" windowWidth="15612" windowHeight="8148" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView visibility="hidden" xWindow="2688" yWindow="2688" windowWidth="34560" windowHeight="19140" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,13 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2">
+        <row r="4">
+          <cell r="B4">
+            <v>0.20807749014095389</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -398,7 +404,13 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2">
+        <row r="4">
+          <cell r="B4">
+            <v>7.092240261140333E-3</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>

<commit_message>
ilemt_calibration_V4.docx and ilemt_calibration_supplemental_V4.docx are pretty much ready to go in (needs proofreading). ilemt_calibration_V4_reply.docx is descriptions of revisions to address issues on the last review cycle.  Also added final report draft.
</commit_message>
<xml_diff>
--- a/calibration/table1_concentric_vs_dipole.xlsx
+++ b/calibration/table1_concentric_vs_dipole.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF843842-264B-4254-A0F8-A9B8560B3EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E1996A-22EB-4C0F-9462-F964B5FFD7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="5760" windowWidth="34560" windowHeight="19140" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="9550" yWindow="3430" windowWidth="28800" windowHeight="15460" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -232,13 +232,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,7 +270,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -295,7 +294,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Error stats"/>
@@ -353,7 +352,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Error stats"/>
@@ -411,9 +410,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -451,7 +450,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -557,7 +556,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -699,7 +698,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -710,61 +709,61 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="10.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
-    <col min="2" max="13" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.6328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="13" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:17" s="12" customFormat="1" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="20" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="17"/>
+      <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="22" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
     </row>
-    <row r="3" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
+    <row r="3" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="18"/>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -802,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -855,7 +854,7 @@
         <v>0.63741010822327027</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -908,81 +907,81 @@
         <v>0.63741010822327027</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:17" s="11" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <f>'[1]Error stats'!B6</f>
         <v>28.325383529852502</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <f t="shared" si="0"/>
         <v>28.325585627012892</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <f>'[1]Error stats'!C6</f>
         <v>73.454045577923338</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <f>'[1]Error stats'!D6</f>
         <v>20.263774989255438</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <f t="shared" si="1"/>
         <v>20.264488071875249</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="15">
         <f>'[1]Error stats'!E6</f>
         <v>56.839424917636663</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f>'[2]Error stats'!F6</f>
         <v>0.90483646095157622</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <f t="shared" si="2"/>
         <v>0.91114105442975912</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <f>'[2]Error stats'!G6</f>
         <v>2.4920522529965377</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <f>'[2]Error stats'!H6</f>
         <v>0.50825270891314323</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <f t="shared" si="3"/>
         <v>0.53592986119225372</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="10">
         <f>'[2]Error stats'!I6</f>
         <v>1.4154726477601904</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>

</xml_diff>

<commit_message>
Final version of calibration paper.
</commit_message>
<xml_diff>
--- a/calibration/table1_concentric_vs_dipole.xlsx
+++ b/calibration/table1_concentric_vs_dipole.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E1996A-22EB-4C0F-9462-F964B5FFD7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFA861E3-3917-4667-BC71-4D509173FDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9550" yWindow="3430" windowWidth="28800" windowHeight="15460" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView visibility="hidden" minimized="1" xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10300" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -403,7 +404,13 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2">
+        <row r="4">
+          <cell r="B4">
+            <v>7.092240261140333E-3</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -863,7 +870,7 @@
         <v>0.17789727827386054</v>
       </c>
       <c r="C5" s="7">
-        <f t="shared" ref="C5:C6" si="0">SQRT(B5^2+0.107^2)</f>
+        <f>SQRT(B5^2+0.107^2)</f>
         <v>0.20759682468006915</v>
       </c>
       <c r="D5" s="7">
@@ -875,7 +882,7 @@
         <v>0.20999540722187857</v>
       </c>
       <c r="F5" s="7">
-        <f t="shared" ref="F5:F6" si="1">SQRT(E5^2+0.17^2)</f>
+        <f>SQRT(E5^2+0.17^2)</f>
         <v>0.27018155202434274</v>
       </c>
       <c r="G5" s="8">
@@ -887,7 +894,7 @@
         <v>0.26305582094218294</v>
       </c>
       <c r="I5" s="7">
-        <f t="shared" ref="I5:I6" si="2">SQRT(H5^2+0.107^2)</f>
+        <f>SQRT(H5^2+0.107^2)</f>
         <v>0.28398479700780782</v>
       </c>
       <c r="J5" s="7">
@@ -899,7 +906,7 @@
         <v>0.27262142803520317</v>
       </c>
       <c r="L5" s="7">
-        <f t="shared" ref="L5:L6" si="3">SQRT(K5^2+0.17^2)</f>
+        <f>SQRT(K5^2+0.17^2)</f>
         <v>0.32128249722627822</v>
       </c>
       <c r="M5" s="7">
@@ -916,7 +923,7 @@
         <v>28.325383529852502</v>
       </c>
       <c r="C6" s="10">
-        <f t="shared" si="0"/>
+        <f>SQRT(B6^2+0.107^2)</f>
         <v>28.325585627012892</v>
       </c>
       <c r="D6" s="14">
@@ -928,7 +935,7 @@
         <v>20.263774989255438</v>
       </c>
       <c r="F6" s="14">
-        <f t="shared" si="1"/>
+        <f>SQRT(E6^2+0.17^2)</f>
         <v>20.264488071875249</v>
       </c>
       <c r="G6" s="15">
@@ -940,7 +947,7 @@
         <v>0.90483646095157622</v>
       </c>
       <c r="I6" s="10">
-        <f t="shared" si="2"/>
+        <f>SQRT(H6^2+0.107^2)</f>
         <v>0.91114105442975912</v>
       </c>
       <c r="J6" s="10">
@@ -952,7 +959,7 @@
         <v>0.50825270891314323</v>
       </c>
       <c r="L6" s="10">
-        <f t="shared" si="3"/>
+        <f>SQRT(K6^2+0.17^2)</f>
         <v>0.53592986119225372</v>
       </c>
       <c r="M6" s="10">

</xml_diff>